<commit_message>
updating the data tracker file
</commit_message>
<xml_diff>
--- a/DataWeHave.xlsx
+++ b/DataWeHave.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="65">
   <si>
     <t>Variable</t>
   </si>
@@ -69,9 +69,6 @@
     <t>per capita income</t>
   </si>
   <si>
-    <t>poverty</t>
-  </si>
-  <si>
     <t>metropolitan GDP</t>
   </si>
   <si>
@@ -84,15 +81,9 @@
     <t>social security</t>
   </si>
   <si>
-    <t>hospitals/health facilities</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
-    <t>air quality</t>
-  </si>
-  <si>
     <t>green space</t>
   </si>
   <si>
@@ -118,6 +109,108 @@
   </si>
   <si>
     <t>FBI</t>
+  </si>
+  <si>
+    <t>:Bachelors degree</t>
+  </si>
+  <si>
+    <t>:%high school grad</t>
+  </si>
+  <si>
+    <t>ACS</t>
+  </si>
+  <si>
+    <t>Median house value</t>
+  </si>
+  <si>
+    <t>% veterans</t>
+  </si>
+  <si>
+    <t>active MDs</t>
+  </si>
+  <si>
+    <t>hospitals</t>
+  </si>
+  <si>
+    <t>AHRF - F12129XX</t>
+  </si>
+  <si>
+    <t>AHRF - F08868XX</t>
+  </si>
+  <si>
+    <t>hospital beds</t>
+  </si>
+  <si>
+    <t>AHRF - F08921XX</t>
+  </si>
+  <si>
+    <t>AHRF - F14084XX</t>
+  </si>
+  <si>
+    <t>Pers &lt;65 W/ insurance</t>
+  </si>
+  <si>
+    <t>Pers &lt;65 W/out insurance</t>
+  </si>
+  <si>
+    <t>AHRF - F14149XX</t>
+  </si>
+  <si>
+    <t>AHRF - F14750XX</t>
+  </si>
+  <si>
+    <t>AHRF - F14159XX</t>
+  </si>
+  <si>
+    <t>household density</t>
+  </si>
+  <si>
+    <t># air quality days measured</t>
+  </si>
+  <si>
+    <t>#good air quality days measured</t>
+  </si>
+  <si>
+    <t># good days</t>
+  </si>
+  <si>
+    <t>AHRF - F15264XX</t>
+  </si>
+  <si>
+    <t>AHRF - F15265XX</t>
+  </si>
+  <si>
+    <t>AHRF - F15266XX</t>
+  </si>
+  <si>
+    <t>AHRF - F13876XX</t>
+  </si>
+  <si>
+    <t>AHRF - F13877XX</t>
+  </si>
+  <si>
+    <t>unemployment</t>
+  </si>
+  <si>
+    <t>AHRF - F06795XX</t>
+  </si>
+  <si>
+    <t># in poverty</t>
+  </si>
+  <si>
+    <t>AHRF - F13223XX</t>
+  </si>
+  <si>
+    <t>AHRF - F13226XX</t>
+  </si>
+  <si>
+    <t>AHRF - F09781XX</t>
+  </si>
+  <si>
+    <t>AHRF - F12557XX</t>
+  </si>
+  <si>
+    <t>AHRF - F14155XX</t>
   </si>
 </sst>
 </file>
@@ -243,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -251,7 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -559,23 +651,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="0.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="24" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -584,7 +675,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1">
@@ -652,7 +743,7 @@
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5"/>
@@ -661,49 +752,49 @@
     <row r="4" spans="1:24" s="4" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="L6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="M6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="N6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="O6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="P6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="S6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -711,10 +802,10 @@
         <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -746,12 +837,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -775,313 +866,633 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" t="s">
-        <v>5</v>
-      </c>
-      <c r="N12" t="s">
-        <v>5</v>
-      </c>
-      <c r="S12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="O13" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="O14" t="s">
+        <v>33</v>
+      </c>
+      <c r="P14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" t="s">
+        <v>61</v>
+      </c>
+      <c r="O19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O21" t="s">
+        <v>33</v>
+      </c>
+      <c r="P21" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" t="s">
+        <v>58</v>
+      </c>
+      <c r="N22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19" t="s">
-        <v>5</v>
-      </c>
-      <c r="K19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" t="s">
-        <v>5</v>
-      </c>
-      <c r="M19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F20" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" t="s">
+        <v>42</v>
+      </c>
+      <c r="M27" t="s">
+        <v>42</v>
+      </c>
+      <c r="N27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" t="s">
+        <v>41</v>
+      </c>
+      <c r="N30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I31" t="s">
+        <v>38</v>
+      </c>
+      <c r="N31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" t="s">
+        <v>45</v>
+      </c>
+      <c r="K32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L32" t="s">
+        <v>47</v>
+      </c>
+      <c r="M32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" t="s">
+        <v>46</v>
+      </c>
+      <c r="L33" t="s">
+        <v>64</v>
+      </c>
+      <c r="M33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="I40" t="s">
+        <v>56</v>
+      </c>
+      <c r="S40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" t="s">
+        <v>30</v>
+      </c>
+      <c r="J42" t="s">
+        <v>30</v>
+      </c>
+      <c r="K42" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" t="s">
+        <v>30</v>
+      </c>
+      <c r="M42" t="s">
+        <v>30</v>
+      </c>
+      <c r="N42" t="s">
+        <v>30</v>
+      </c>
+      <c r="O42" t="s">
+        <v>30</v>
+      </c>
+      <c r="P42" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>30</v>
+      </c>
+      <c r="R42" t="s">
+        <v>30</v>
+      </c>
+      <c r="S42" t="s">
+        <v>30</v>
+      </c>
+      <c r="T42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>28</v>
       </c>
-      <c r="G20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" t="s">
+        <v>30</v>
+      </c>
+      <c r="J43" t="s">
+        <v>30</v>
+      </c>
+      <c r="K43" t="s">
+        <v>30</v>
+      </c>
+      <c r="L43" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" t="s">
+        <v>30</v>
+      </c>
+      <c r="N43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" t="s">
+        <v>30</v>
+      </c>
+      <c r="P43" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>30</v>
+      </c>
+      <c r="R43" t="s">
+        <v>30</v>
+      </c>
+      <c r="S43" t="s">
+        <v>30</v>
+      </c>
+      <c r="T43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>29</v>
       </c>
-      <c r="F21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" t="s">
-        <v>33</v>
-      </c>
-      <c r="L30" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O30" t="s">
-        <v>33</v>
-      </c>
-      <c r="P30" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>33</v>
-      </c>
-      <c r="R30" t="s">
-        <v>33</v>
-      </c>
-      <c r="S30" t="s">
-        <v>33</v>
-      </c>
-      <c r="T30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" t="s">
-        <v>33</v>
-      </c>
-      <c r="I31" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" t="s">
-        <v>33</v>
-      </c>
-      <c r="K31" t="s">
-        <v>33</v>
-      </c>
-      <c r="L31" t="s">
-        <v>33</v>
-      </c>
-      <c r="M31" t="s">
-        <v>33</v>
-      </c>
-      <c r="N31" t="s">
-        <v>33</v>
-      </c>
-      <c r="O31" t="s">
-        <v>33</v>
-      </c>
-      <c r="P31" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>33</v>
-      </c>
-      <c r="R31" t="s">
-        <v>33</v>
-      </c>
-      <c r="S31" t="s">
-        <v>33</v>
-      </c>
-      <c r="T31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K32" t="s">
-        <v>33</v>
-      </c>
-      <c r="L32" t="s">
-        <v>33</v>
-      </c>
-      <c r="M32" t="s">
-        <v>33</v>
-      </c>
-      <c r="N32" t="s">
-        <v>33</v>
-      </c>
-      <c r="O32" t="s">
-        <v>33</v>
-      </c>
-      <c r="P32" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>33</v>
-      </c>
-      <c r="R32" t="s">
-        <v>33</v>
-      </c>
-      <c r="S32" t="s">
-        <v>33</v>
-      </c>
-      <c r="T32" t="s">
-        <v>33</v>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" t="s">
+        <v>30</v>
+      </c>
+      <c r="I44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J44" t="s">
+        <v>30</v>
+      </c>
+      <c r="K44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L44" t="s">
+        <v>30</v>
+      </c>
+      <c r="M44" t="s">
+        <v>30</v>
+      </c>
+      <c r="N44" t="s">
+        <v>30</v>
+      </c>
+      <c r="O44" t="s">
+        <v>30</v>
+      </c>
+      <c r="P44" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>30</v>
+      </c>
+      <c r="R44" t="s">
+        <v>30</v>
+      </c>
+      <c r="S44" t="s">
+        <v>30</v>
+      </c>
+      <c r="T44" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another update of data we have
</commit_message>
<xml_diff>
--- a/DataWeHave.xlsx
+++ b/DataWeHave.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="71">
   <si>
     <t>Variable</t>
   </si>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -960,14 +960,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>57</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>59</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -1141,15 +1141,51 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="F25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" t="s">
+        <v>25</v>
+      </c>
+      <c r="O25" t="s">
+        <v>25</v>
+      </c>
+      <c r="P25" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>25</v>
+      </c>
+      <c r="R25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>65</v>
       </c>
@@ -1169,14 +1205,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="12"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>19</v>
       </c>
@@ -1202,12 +1238,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>37</v>
       </c>
@@ -1221,7 +1257,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>40</v>
       </c>
@@ -1232,7 +1268,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>36</v>
       </c>

</xml_diff>